<commit_message>
tambah func ambil data excel
</commit_message>
<xml_diff>
--- a/data_obat.xlsx
+++ b/data_obat.xlsx
@@ -43,10 +43,10 @@
     <t>paracetamol</t>
   </si>
   <si>
-    <t>narkotika</t>
-  </si>
-  <si>
-    <t>Berat</t>
+    <t>kapsul</t>
+  </si>
+  <si>
+    <t>keras</t>
   </si>
   <si>
     <t>Bebas</t>
@@ -55,7 +55,7 @@
     <t>B</t>
   </si>
   <si>
-    <t>22/06/2025</t>
+    <t>28/06/2045</t>
   </si>
 </sst>
 </file>
@@ -401,10 +401,10 @@
         <v>10</v>
       </c>
       <c r="D2">
-        <v>11000</v>
+        <v>20000</v>
       </c>
       <c r="E2">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>

</xml_diff>